<commit_message>
adds more documentation; cleans, organizes, and sorts code; adds growth rates to kpis
</commit_message>
<xml_diff>
--- a/Insight-Dataset/KPI-Dataset.xlsx
+++ b/Insight-Dataset/KPI-Dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,32 +441,72 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Total_Revenue</t>
+          <t>total_revenue</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Number_of_Orders</t>
+          <t>revenue_growth_rate</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Unique_Customers_Who_Made_a_Purchase</t>
+          <t>number_of_orders</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>New_Customers</t>
+          <t>number_of_items</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Total_Customers</t>
+          <t>unique_customers_who_made_a_purchase</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Average_Customer_Lifespan_in_Days</t>
+          <t>new_customers</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>total_customers</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>average_customer_lifespan_in_days</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>new_customer_growth_rate</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>new_sellers</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>total_sellers</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>average_sellers_lifespan_in_days</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>unique_sellers_who_made_a_sell</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>new_seller_growth_rate</t>
         </is>
       </c>
     </row>
@@ -480,19 +520,43 @@
         <v>121884</v>
       </c>
       <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
         <v>715</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
+        <v>869</v>
+      </c>
+      <c r="F2" t="n">
         <v>684</v>
       </c>
-      <c r="E2" t="n">
-        <v>683</v>
-      </c>
-      <c r="F2" t="n">
-        <v>683</v>
-      </c>
       <c r="G2" t="n">
-        <v>1.002928257686676</v>
+        <v>684</v>
+      </c>
+      <c r="H2" t="n">
+        <v>684</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.001461988304094</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>213</v>
+      </c>
+      <c r="L2" t="n">
+        <v>213</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4.676056338028169</v>
+      </c>
+      <c r="N2" t="n">
+        <v>213</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -505,19 +569,43 @@
         <v>270749</v>
       </c>
       <c r="C3" t="n">
+        <v>122.1366217058843</v>
+      </c>
+      <c r="D3" t="n">
         <v>1638</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
+        <v>1838</v>
+      </c>
+      <c r="F3" t="n">
         <v>1615</v>
       </c>
-      <c r="E3" t="n">
-        <v>1605</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2288</v>
-      </c>
       <c r="G3" t="n">
-        <v>0.7456293706293706</v>
+        <v>1612</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2296</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.7430313588850174</v>
+      </c>
+      <c r="J3" t="n">
+        <v>135.672514619883</v>
+      </c>
+      <c r="K3" t="n">
+        <v>240</v>
+      </c>
+      <c r="L3" t="n">
+        <v>453</v>
+      </c>
+      <c r="M3" t="n">
+        <v>13.30684326710817</v>
+      </c>
+      <c r="N3" t="n">
+        <v>405</v>
+      </c>
+      <c r="O3" t="n">
+        <v>12.67605633802817</v>
       </c>
     </row>
     <row r="4">
@@ -530,19 +618,43 @@
         <v>410734</v>
       </c>
       <c r="C4" t="n">
+        <v>51.70286870865636</v>
+      </c>
+      <c r="D4" t="n">
         <v>2554</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
+        <v>2918</v>
+      </c>
+      <c r="F4" t="n">
         <v>2516</v>
       </c>
-      <c r="E4" t="n">
-        <v>2507</v>
-      </c>
-      <c r="F4" t="n">
-        <v>4795</v>
-      </c>
       <c r="G4" t="n">
-        <v>0.5635036496350365</v>
+        <v>2511</v>
+      </c>
+      <c r="H4" t="n">
+        <v>4807</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.5620969419596422</v>
+      </c>
+      <c r="J4" t="n">
+        <v>55.76923076923077</v>
+      </c>
+      <c r="K4" t="n">
+        <v>165</v>
+      </c>
+      <c r="L4" t="n">
+        <v>618</v>
+      </c>
+      <c r="M4" t="n">
+        <v>26.48867313915857</v>
+      </c>
+      <c r="N4" t="n">
+        <v>478</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-31.25</v>
       </c>
     </row>
     <row r="5">
@@ -555,19 +667,43 @@
         <v>387782</v>
       </c>
       <c r="C5" t="n">
+        <v>-5.588044817327029</v>
+      </c>
+      <c r="D5" t="n">
         <v>2278</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
+        <v>2540</v>
+      </c>
+      <c r="F5" t="n">
         <v>2249</v>
       </c>
-      <c r="E5" t="n">
-        <v>2229</v>
-      </c>
-      <c r="F5" t="n">
-        <v>7024</v>
-      </c>
       <c r="G5" t="n">
-        <v>0.4164293849658314</v>
+        <v>2233</v>
+      </c>
+      <c r="H5" t="n">
+        <v>7040</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.4154829545454545</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-11.07128634010354</v>
+      </c>
+      <c r="K5" t="n">
+        <v>115</v>
+      </c>
+      <c r="L5" t="n">
+        <v>733</v>
+      </c>
+      <c r="M5" t="n">
+        <v>35.07366984993179</v>
+      </c>
+      <c r="N5" t="n">
+        <v>487</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-30.3030303030303</v>
       </c>
     </row>
     <row r="6">
@@ -580,19 +716,43 @@
         <v>568069</v>
       </c>
       <c r="C6" t="n">
+        <v>46.49184335528725</v>
+      </c>
+      <c r="D6" t="n">
         <v>3548</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
+        <v>3999</v>
+      </c>
+      <c r="F6" t="n">
         <v>3482</v>
       </c>
-      <c r="E6" t="n">
-        <v>3434</v>
-      </c>
-      <c r="F6" t="n">
-        <v>10458</v>
-      </c>
       <c r="G6" t="n">
-        <v>0.4914897685982023</v>
+        <v>3453</v>
+      </c>
+      <c r="H6" t="n">
+        <v>10493</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.4898503764414371</v>
+      </c>
+      <c r="J6" t="n">
+        <v>54.63502015226153</v>
+      </c>
+      <c r="K6" t="n">
+        <v>116</v>
+      </c>
+      <c r="L6" t="n">
+        <v>849</v>
+      </c>
+      <c r="M6" t="n">
+        <v>48.42167255594818</v>
+      </c>
+      <c r="N6" t="n">
+        <v>562</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.8695652173913043</v>
       </c>
     </row>
     <row r="7">
@@ -605,19 +765,43 @@
         <v>494351</v>
       </c>
       <c r="C7" t="n">
+        <v>-12.97694470214006</v>
+      </c>
+      <c r="D7" t="n">
         <v>3143</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
+        <v>3505</v>
+      </c>
+      <c r="F7" t="n">
         <v>3084</v>
       </c>
-      <c r="E7" t="n">
-        <v>3033</v>
-      </c>
-      <c r="F7" t="n">
-        <v>13491</v>
-      </c>
       <c r="G7" t="n">
-        <v>0.4166481357942332</v>
+        <v>3044</v>
+      </c>
+      <c r="H7" t="n">
+        <v>13537</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.4152323262170348</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-11.84477266145381</v>
+      </c>
+      <c r="K7" t="n">
+        <v>69</v>
+      </c>
+      <c r="L7" t="n">
+        <v>918</v>
+      </c>
+      <c r="M7" t="n">
+        <v>54.02614379084967</v>
+      </c>
+      <c r="N7" t="n">
+        <v>519</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-40.51724137931034</v>
       </c>
     </row>
     <row r="8">
@@ -630,19 +814,43 @@
         <v>560275</v>
       </c>
       <c r="C8" t="n">
+        <v>13.33546407309786</v>
+      </c>
+      <c r="D8" t="n">
         <v>3828</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
+        <v>4364</v>
+      </c>
+      <c r="F8" t="n">
         <v>3759</v>
       </c>
-      <c r="E8" t="n">
-        <v>3696</v>
-      </c>
-      <c r="F8" t="n">
-        <v>17187</v>
-      </c>
       <c r="G8" t="n">
-        <v>0.4409728283004596</v>
+        <v>3710</v>
+      </c>
+      <c r="H8" t="n">
+        <v>17247</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.4394387429697919</v>
+      </c>
+      <c r="J8" t="n">
+        <v>21.87910643889619</v>
+      </c>
+      <c r="K8" t="n">
+        <v>112</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1030</v>
+      </c>
+      <c r="M8" t="n">
+        <v>62.32718446601942</v>
+      </c>
+      <c r="N8" t="n">
+        <v>587</v>
+      </c>
+      <c r="O8" t="n">
+        <v>62.31884057971014</v>
       </c>
     </row>
     <row r="9">
@@ -655,19 +863,43 @@
         <v>646567</v>
       </c>
       <c r="C9" t="n">
+        <v>15.40172236847976</v>
+      </c>
+      <c r="D9" t="n">
         <v>4217</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
+        <v>4824</v>
+      </c>
+      <c r="F9" t="n">
         <v>4137</v>
       </c>
-      <c r="E9" t="n">
-        <v>4068</v>
-      </c>
-      <c r="F9" t="n">
-        <v>21255</v>
-      </c>
       <c r="G9" t="n">
-        <v>0.4031521994824747</v>
+        <v>4081</v>
+      </c>
+      <c r="H9" t="n">
+        <v>21328</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.4017723180795199</v>
+      </c>
+      <c r="J9" t="n">
+        <v>10</v>
+      </c>
+      <c r="K9" t="n">
+        <v>123</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1153</v>
+      </c>
+      <c r="M9" t="n">
+        <v>72.78404163052906</v>
+      </c>
+      <c r="N9" t="n">
+        <v>685</v>
+      </c>
+      <c r="O9" t="n">
+        <v>9.821428571428571</v>
       </c>
     </row>
     <row r="10">
@@ -680,19 +912,43 @@
         <v>691353</v>
       </c>
       <c r="C10" t="n">
+        <v>6.926737677611137</v>
+      </c>
+      <c r="D10" t="n">
         <v>4170</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
+        <v>4757</v>
+      </c>
+      <c r="F10" t="n">
         <v>4103</v>
       </c>
-      <c r="E10" t="n">
-        <v>4008</v>
-      </c>
-      <c r="F10" t="n">
-        <v>25263</v>
-      </c>
       <c r="G10" t="n">
-        <v>0.4242172346910502</v>
+        <v>4026</v>
+      </c>
+      <c r="H10" t="n">
+        <v>25354</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.4226946438431806</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-1.347708894878706</v>
+      </c>
+      <c r="K10" t="n">
+        <v>124</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1277</v>
+      </c>
+      <c r="M10" t="n">
+        <v>74.0602975724354</v>
+      </c>
+      <c r="N10" t="n">
+        <v>712</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.8130081300813009</v>
       </c>
     </row>
     <row r="11">
@@ -705,19 +961,43 @@
         <v>755320</v>
       </c>
       <c r="C11" t="n">
+        <v>9.252436888246669</v>
+      </c>
+      <c r="D11" t="n">
         <v>4441</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
+        <v>5165</v>
+      </c>
+      <c r="F11" t="n">
         <v>4380</v>
       </c>
-      <c r="E11" t="n">
-        <v>4284</v>
-      </c>
-      <c r="F11" t="n">
-        <v>29547</v>
-      </c>
       <c r="G11" t="n">
-        <v>0.4320574000744576</v>
+        <v>4294</v>
+      </c>
+      <c r="H11" t="n">
+        <v>29648</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.4305855369670804</v>
+      </c>
+      <c r="J11" t="n">
+        <v>6.656731246895181</v>
+      </c>
+      <c r="K11" t="n">
+        <v>138</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1415</v>
+      </c>
+      <c r="M11" t="n">
+        <v>78.71095406360423</v>
+      </c>
+      <c r="N11" t="n">
+        <v>758</v>
+      </c>
+      <c r="O11" t="n">
+        <v>11.29032258064516</v>
       </c>
     </row>
     <row r="12">
@@ -730,19 +1010,43 @@
         <v>1135057</v>
       </c>
       <c r="C12" t="n">
+        <v>50.27498278875179</v>
+      </c>
+      <c r="D12" t="n">
         <v>7150</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
+        <v>8323</v>
+      </c>
+      <c r="F12" t="n">
         <v>7045</v>
       </c>
-      <c r="E12" t="n">
-        <v>6906</v>
-      </c>
-      <c r="F12" t="n">
-        <v>36453</v>
-      </c>
       <c r="G12" t="n">
-        <v>0.5656050256494665</v>
+        <v>6928</v>
+      </c>
+      <c r="H12" t="n">
+        <v>36576</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.5637029746281714</v>
+      </c>
+      <c r="J12" t="n">
+        <v>61.34140661387983</v>
+      </c>
+      <c r="K12" t="n">
+        <v>187</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1602</v>
+      </c>
+      <c r="M12" t="n">
+        <v>87.54057428214732</v>
+      </c>
+      <c r="N12" t="n">
+        <v>933</v>
+      </c>
+      <c r="O12" t="n">
+        <v>35.50724637681159</v>
       </c>
     </row>
     <row r="13">
@@ -755,19 +1059,43 @@
         <v>867940</v>
       </c>
       <c r="C13" t="n">
+        <v>-23.53335559359574</v>
+      </c>
+      <c r="D13" t="n">
         <v>5675</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
+        <v>6378</v>
+      </c>
+      <c r="F13" t="n">
         <v>5608</v>
       </c>
-      <c r="E13" t="n">
-        <v>5474</v>
-      </c>
-      <c r="F13" t="n">
-        <v>41927</v>
-      </c>
       <c r="G13" t="n">
-        <v>0.4283397333460539</v>
+        <v>5490</v>
+      </c>
+      <c r="H13" t="n">
+        <v>42066</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.4269243569628679</v>
+      </c>
+      <c r="J13" t="n">
+        <v>-20.75635103926097</v>
+      </c>
+      <c r="K13" t="n">
+        <v>88</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1690</v>
+      </c>
+      <c r="M13" t="n">
+        <v>87.51715976331361</v>
+      </c>
+      <c r="N13" t="n">
+        <v>860</v>
+      </c>
+      <c r="O13" t="n">
+        <v>-52.94117647058824</v>
       </c>
     </row>
     <row r="14">
@@ -780,19 +1108,43 @@
         <v>1069384</v>
       </c>
       <c r="C14" t="n">
+        <v>23.20943844044519</v>
+      </c>
+      <c r="D14" t="n">
         <v>6991</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
+        <v>7931</v>
+      </c>
+      <c r="F14" t="n">
         <v>6901</v>
       </c>
-      <c r="E14" t="n">
-        <v>6750</v>
-      </c>
-      <c r="F14" t="n">
-        <v>48677</v>
-      </c>
       <c r="G14" t="n">
-        <v>0.5648252768247838</v>
+        <v>6771</v>
+      </c>
+      <c r="H14" t="n">
+        <v>48837</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.5629747937014968</v>
+      </c>
+      <c r="J14" t="n">
+        <v>23.33333333333333</v>
+      </c>
+      <c r="K14" t="n">
+        <v>136</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1826</v>
+      </c>
+      <c r="M14" t="n">
+        <v>95.00438116100767</v>
+      </c>
+      <c r="N14" t="n">
+        <v>955</v>
+      </c>
+      <c r="O14" t="n">
+        <v>54.54545454545454</v>
       </c>
     </row>
     <row r="15">
@@ -805,19 +1157,43 @@
         <v>958364</v>
       </c>
       <c r="C15" t="n">
+        <v>-10.38167767612008</v>
+      </c>
+      <c r="D15" t="n">
         <v>6536</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
+        <v>7504</v>
+      </c>
+      <c r="F15" t="n">
         <v>6380</v>
       </c>
-      <c r="E15" t="n">
-        <v>6249</v>
-      </c>
-      <c r="F15" t="n">
-        <v>54926</v>
-      </c>
       <c r="G15" t="n">
-        <v>0.4069839420310964</v>
+        <v>6268</v>
+      </c>
+      <c r="H15" t="n">
+        <v>55105</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.4056619181562472</v>
+      </c>
+      <c r="J15" t="n">
+        <v>-7.428740215625461</v>
+      </c>
+      <c r="K15" t="n">
+        <v>117</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1943</v>
+      </c>
+      <c r="M15" t="n">
+        <v>93.95419454451878</v>
+      </c>
+      <c r="N15" t="n">
+        <v>929</v>
+      </c>
+      <c r="O15" t="n">
+        <v>-13.97058823529412</v>
       </c>
     </row>
     <row r="16">
@@ -830,19 +1206,43 @@
         <v>1132427</v>
       </c>
       <c r="C16" t="n">
+        <v>18.16251445171146</v>
+      </c>
+      <c r="D16" t="n">
         <v>7083</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
+        <v>8107</v>
+      </c>
+      <c r="F16" t="n">
         <v>6989</v>
       </c>
-      <c r="E16" t="n">
-        <v>6834</v>
-      </c>
-      <c r="F16" t="n">
-        <v>61760</v>
-      </c>
       <c r="G16" t="n">
-        <v>0.4444300518134715</v>
+        <v>6852</v>
+      </c>
+      <c r="H16" t="n">
+        <v>61957</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.443016931097374</v>
+      </c>
+      <c r="J16" t="n">
+        <v>9.317166560306319</v>
+      </c>
+      <c r="K16" t="n">
+        <v>110</v>
+      </c>
+      <c r="L16" t="n">
+        <v>2053</v>
+      </c>
+      <c r="M16" t="n">
+        <v>102.2075012177302</v>
+      </c>
+      <c r="N16" t="n">
+        <v>987</v>
+      </c>
+      <c r="O16" t="n">
+        <v>-5.982905982905983</v>
       </c>
     </row>
     <row r="17">
@@ -855,19 +1255,43 @@
         <v>1109550</v>
       </c>
       <c r="C17" t="n">
+        <v>-2.020174368855564</v>
+      </c>
+      <c r="D17" t="n">
         <v>6639</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
+        <v>7640</v>
+      </c>
+      <c r="F17" t="n">
         <v>6586</v>
       </c>
-      <c r="E17" t="n">
-        <v>6409</v>
-      </c>
-      <c r="F17" t="n">
-        <v>68169</v>
-      </c>
       <c r="G17" t="n">
-        <v>0.4532558787718758</v>
+        <v>6428</v>
+      </c>
+      <c r="H17" t="n">
+        <v>68385</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.4518242304598962</v>
+      </c>
+      <c r="J17" t="n">
+        <v>-6.187974314068885</v>
+      </c>
+      <c r="K17" t="n">
+        <v>192</v>
+      </c>
+      <c r="L17" t="n">
+        <v>2245</v>
+      </c>
+      <c r="M17" t="n">
+        <v>101.4004454342984</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1095</v>
+      </c>
+      <c r="O17" t="n">
+        <v>74.54545454545455</v>
       </c>
     </row>
     <row r="18">
@@ -880,19 +1304,43 @@
         <v>1155339</v>
       </c>
       <c r="C18" t="n">
+        <v>4.126808165472489</v>
+      </c>
+      <c r="D18" t="n">
         <v>6940</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
+        <v>8041</v>
+      </c>
+      <c r="F18" t="n">
         <v>6884</v>
       </c>
-      <c r="E18" t="n">
-        <v>6666</v>
-      </c>
-      <c r="F18" t="n">
-        <v>74835</v>
-      </c>
       <c r="G18" t="n">
-        <v>0.4888087125008352</v>
+        <v>6694</v>
+      </c>
+      <c r="H18" t="n">
+        <v>75079</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.4872201281317013</v>
+      </c>
+      <c r="J18" t="n">
+        <v>4.138145612943372</v>
+      </c>
+      <c r="K18" t="n">
+        <v>174</v>
+      </c>
+      <c r="L18" t="n">
+        <v>2419</v>
+      </c>
+      <c r="M18" t="n">
+        <v>96.88466308391898</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1114</v>
+      </c>
+      <c r="O18" t="n">
+        <v>-9.375</v>
       </c>
     </row>
     <row r="19">
@@ -905,19 +1353,43 @@
         <v>1015534</v>
       </c>
       <c r="C19" t="n">
+        <v>-12.10077734760101</v>
+      </c>
+      <c r="D19" t="n">
         <v>6097</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
+        <v>7002</v>
+      </c>
+      <c r="F19" t="n">
         <v>6060</v>
       </c>
-      <c r="E19" t="n">
-        <v>5863</v>
-      </c>
-      <c r="F19" t="n">
-        <v>80698</v>
-      </c>
       <c r="G19" t="n">
-        <v>0.4684502713821904</v>
+        <v>5876</v>
+      </c>
+      <c r="H19" t="n">
+        <v>80955</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.4669631276635168</v>
+      </c>
+      <c r="J19" t="n">
+        <v>-12.21989841649238</v>
+      </c>
+      <c r="K19" t="n">
+        <v>188</v>
+      </c>
+      <c r="L19" t="n">
+        <v>2607</v>
+      </c>
+      <c r="M19" t="n">
+        <v>97.30571538166475</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1167</v>
+      </c>
+      <c r="O19" t="n">
+        <v>8.045977011494253</v>
       </c>
     </row>
     <row r="20">
@@ -930,19 +1402,43 @@
         <v>1006421</v>
       </c>
       <c r="C20" t="n">
+        <v>-0.8973604034921528</v>
+      </c>
+      <c r="D20" t="n">
         <v>6050</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
+        <v>6830</v>
+      </c>
+      <c r="F20" t="n">
         <v>5991</v>
       </c>
-      <c r="E20" t="n">
-        <v>5832</v>
-      </c>
-      <c r="F20" t="n">
-        <v>86530</v>
-      </c>
       <c r="G20" t="n">
-        <v>0.3880388304634231</v>
+        <v>5846</v>
+      </c>
+      <c r="H20" t="n">
+        <v>86801</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.3868273406988399</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-0.5105513955071478</v>
+      </c>
+      <c r="K20" t="n">
+        <v>180</v>
+      </c>
+      <c r="L20" t="n">
+        <v>2787</v>
+      </c>
+      <c r="M20" t="n">
+        <v>98.9519196268389</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1228</v>
+      </c>
+      <c r="O20" t="n">
+        <v>-4.25531914893617</v>
       </c>
     </row>
     <row r="21">
@@ -955,19 +1451,43 @@
         <v>1014055</v>
       </c>
       <c r="C21" t="n">
+        <v>0.758529482194827</v>
+      </c>
+      <c r="D21" t="n">
         <v>6504</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
+        <v>7330</v>
+      </c>
+      <c r="F21" t="n">
         <v>6459</v>
       </c>
-      <c r="E21" t="n">
-        <v>6268</v>
-      </c>
-      <c r="F21" t="n">
-        <v>92798</v>
-      </c>
       <c r="G21" t="n">
-        <v>0.4306450570055389</v>
+        <v>6290</v>
+      </c>
+      <c r="H21" t="n">
+        <v>93091</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.4292896198343557</v>
+      </c>
+      <c r="J21" t="n">
+        <v>7.59493670886076</v>
+      </c>
+      <c r="K21" t="n">
+        <v>158</v>
+      </c>
+      <c r="L21" t="n">
+        <v>2945</v>
+      </c>
+      <c r="M21" t="n">
+        <v>99.89575551782683</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1269</v>
+      </c>
+      <c r="O21" t="n">
+        <v>-12.22222222222222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>